<commit_message>
Adicionei a documentação, ainda falta completar e adicionar fotos e outras imagens
</commit_message>
<xml_diff>
--- a/BACKLOG - Nippon Insight.xlsx
+++ b/BACKLOG - Nippon Insight.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0C59508-8A90-49DA-8D15-0478C9C03467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\Projeto Individual\projeto_nippon_insight\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC4FA57-C643-4F66-B6AE-B988986134EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG" sheetId="1" r:id="rId1"/>
@@ -1014,7 +1019,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1053,22 +1058,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1127,6 +1116,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFDB7F42"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1200,7 +1197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1240,22 +1237,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1295,7 +1282,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -1303,7 +1290,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -1311,82 +1298,67 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -1394,6 +1366,25 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1401,11 +1392,21 @@
   <dxfs count="15">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFCC2C9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1421,11 +1422,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFCC2C9"/>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1474,8 +1475,28 @@
         <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFAD2DE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFB0630B"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFAE8CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF0A5C5E"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFA3E3E6"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1519,40 +1540,13 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0A5C5E"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFA3E3E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFB0630B"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFAE8CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFAD2DE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF0BC1BD"/>
+      <color rgb="FF0DDCD7"/>
+      <color rgb="FFE46297"/>
       <color rgb="FFB0630B"/>
       <color rgb="FFFAE8CD"/>
       <color rgb="FFA1850B"/>
@@ -1560,9 +1554,6 @@
       <color rgb="FFD17A0F"/>
       <color rgb="FFFAF1CD"/>
       <color rgb="FFA3E3E6"/>
-      <color rgb="FF0A5C5E"/>
-      <color rgb="FF108D91"/>
-      <color rgb="FFAFEBED"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1668,7 +1659,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="D86DCD"/>
+                <a:srgbClr val="E46297"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
               <a:round/>
@@ -1749,7 +1740,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="0F9ED5"/>
+                <a:srgbClr val="0DDCD7"/>
               </a:solidFill>
               <a:prstDash val="solid"/>
               <a:round/>
@@ -1759,6 +1750,28 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="28575" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="0BC1BD"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-FAA1-487F-9539-FEB18C970F86}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>BACKLOG!$N$2:$N$6</c:f>
@@ -1789,10 +1802,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3136,81 +3149,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="0.39997558519241921"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.88671875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="18" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="18" style="2" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="16" style="2" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" style="2" customWidth="1"/>
     <col min="15" max="15" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="21" width="9.140625" style="2" customWidth="1"/>
+    <col min="18" max="21" width="9.109375" style="2" customWidth="1"/>
     <col min="22" max="16384" width="0" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="36" customFormat="1" ht="15.75">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:17" s="32" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="J1" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="58"/>
-      <c r="L1" s="18" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="O1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="50" t="s">
+      <c r="P1" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="48" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75">
+    <row r="2" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>13</v>
       </c>
@@ -3239,86 +3253,86 @@
       <c r="I2" s="13">
         <v>45964</v>
       </c>
-      <c r="J2" s="61" t="b">
+      <c r="J2" s="52" t="b">
         <f>IF(K2="","",TRUE)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="59">
+      <c r="K2" s="50">
         <v>45962</v>
       </c>
-      <c r="L2" s="34" t="b">
+      <c r="L2" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="N2" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="49">
+      <c r="O2" s="45">
         <f>SUM(O3:O6)</f>
         <v>358</v>
       </c>
-      <c r="P2" s="51">
+      <c r="P2" s="47">
         <f t="shared" ref="P2:Q2" si="0">SUM(P3:P6)</f>
-        <v>55</v>
-      </c>
-      <c r="Q2" s="53">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="49">
         <f t="shared" si="0"/>
-        <v>303</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="18">
         <v>2</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="18">
         <v>1</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="20">
         <f>IF(F3="","",_xlfn.XLOOKUP(F3,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>13</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="20">
         <v>2</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="21">
         <v>45971</v>
       </c>
-      <c r="J3" s="61" t="str">
+      <c r="J3" s="52" t="str">
         <f t="shared" ref="J3:J40" si="1">IF(K3="","",TRUE)</f>
         <v/>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="35" t="b">
+      <c r="K3" s="51"/>
+      <c r="L3" s="31" t="b">
         <v>0</v>
       </c>
-      <c r="N3" s="44">
+      <c r="N3" s="40">
         <v>45964</v>
       </c>
-      <c r="O3" s="45">
+      <c r="O3" s="41">
         <f>SUMPRODUCT(SUMIF($I$2:$I$40,N3,$G$2:$G$40))</f>
         <v>50</v>
       </c>
-      <c r="P3" s="45">
+      <c r="P3" s="41">
         <f>SUMPRODUCT(SUMIFS($G$2:$G$40,$K$2:$K$40,"&lt;="&amp;N3,$J$2:$J$40,TRUE))</f>
-        <v>55</v>
-      </c>
-      <c r="Q3" s="46">
+        <v>63</v>
+      </c>
+      <c r="Q3" s="42">
         <f>O3-(SUMPRODUCT(SUMIFS($G$2:$G$40,$I$2:$I$40,N3,$J$2:$J$40,TRUE)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="20.25" customHeight="1">
+    <row r="4" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="57"/>
       <c r="B4" s="11">
         <v>2</v>
@@ -3345,82 +3359,84 @@
       <c r="I4" s="13">
         <v>45971</v>
       </c>
-      <c r="J4" s="61" t="str">
+      <c r="J4" s="52" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K4" s="50">
+        <v>45964</v>
+      </c>
+      <c r="L4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="35">
+        <v>45971</v>
+      </c>
+      <c r="O4" s="43">
+        <f t="shared" ref="O4:O6" si="2">SUMPRODUCT(SUMIF($I$2:$I$40,N4,$G$2:$G$40))</f>
+        <v>68</v>
+      </c>
+      <c r="P4" s="44">
+        <f>SUMPRODUCT(SUMIFS($G$2:$G$40,$K$2:$K$40,"&gt;"&amp;N3,$K$2:$K$40,"&lt;="&amp;N4,$J$2:$J$40,TRUE))</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="44">
+        <f t="shared" ref="Q4:Q6" si="3">O4-(SUMPRODUCT(SUMIFS($G$2:$G$40,$I$2:$I$40,N4,$J$2:$J$40,TRUE)))</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="57"/>
+      <c r="B5" s="22">
+        <v>2</v>
+      </c>
+      <c r="C5" s="22">
+        <v>3</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="20">
+        <f>IF(F5="","",_xlfn.XLOOKUP(F5,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
+        <v>5</v>
+      </c>
+      <c r="H5" s="20">
+        <v>3</v>
+      </c>
+      <c r="I5" s="21">
+        <v>45978</v>
+      </c>
+      <c r="J5" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K4" s="59"/>
-      <c r="L4" s="34" t="b">
-        <v>0</v>
-      </c>
-      <c r="N4" s="39">
-        <v>45971</v>
-      </c>
-      <c r="O4" s="47">
-        <f t="shared" ref="O4:O6" si="2">SUMPRODUCT(SUMIF($I$2:$I$40,N4,$G$2:$G$40))</f>
-        <v>68</v>
-      </c>
-      <c r="P4" s="48">
-        <f>SUMPRODUCT(SUMIFS($G$2:$G$40,$K$2:$K$40,"&gt;"&amp;N3,$K$2:$K$40,"&lt;="&amp;N4,$J$2:$J$40,TRUE))</f>
-        <v>0</v>
-      </c>
-      <c r="Q4" s="48">
-        <f t="shared" ref="Q4:Q6" si="3">O4-(SUMPRODUCT(SUMIFS($G$2:$G$40,$I$2:$I$40,N4,$J$2:$J$40,TRUE)))</f>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A5" s="57"/>
-      <c r="B5" s="26">
-        <v>2</v>
-      </c>
-      <c r="C5" s="26">
-        <v>3</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="24">
-        <f>IF(F5="","",_xlfn.XLOOKUP(F5,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
-      </c>
-      <c r="H5" s="24">
-        <v>3</v>
-      </c>
-      <c r="I5" s="25">
-        <v>45978</v>
-      </c>
-      <c r="J5" s="61" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K5" s="60"/>
-      <c r="L5" s="35" t="b">
+      <c r="K5" s="51"/>
+      <c r="L5" s="31" t="b">
         <v>0</v>
       </c>
       <c r="N5" s="13">
         <v>45978</v>
       </c>
-      <c r="O5" s="42">
+      <c r="O5" s="38">
         <f>SUMPRODUCT(SUMIF($I$2:$I$40,N5,$G$2:$G$40))</f>
         <v>133</v>
       </c>
-      <c r="P5" s="43">
+      <c r="P5" s="39">
         <f t="shared" ref="P5:P6" si="4">SUMPRODUCT(SUMIFS($G$2:$G$40,$K$2:$K$40,"&gt;"&amp;N4,$K$2:$K$40,"&lt;="&amp;N5,$J$2:$J$40,TRUE))</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="43">
+      <c r="Q5" s="39">
         <f t="shared" si="3"/>
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="19.5" customHeight="1">
+    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56" t="s">
         <v>25</v>
       </c>
@@ -3449,86 +3465,86 @@
       <c r="I6" s="13">
         <v>45964</v>
       </c>
-      <c r="J6" s="61" t="b">
+      <c r="J6" s="52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K6" s="59">
+      <c r="K6" s="50">
         <v>45962</v>
       </c>
-      <c r="L6" s="34" t="b">
+      <c r="L6" s="30" t="b">
         <v>1</v>
       </c>
       <c r="N6" s="13">
         <v>45985</v>
       </c>
-      <c r="O6" s="40">
+      <c r="O6" s="36">
         <f t="shared" si="2"/>
         <v>107</v>
       </c>
-      <c r="P6" s="41">
+      <c r="P6" s="37">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="41">
+      <c r="Q6" s="37">
         <f t="shared" si="3"/>
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75">
+    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="56"/>
-      <c r="B7" s="26">
+      <c r="B7" s="22">
         <v>3</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="22">
         <v>2</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="24" t="s">
+      <c r="F7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="20">
         <f>IF(F7="","",_xlfn.XLOOKUP(F7,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>5</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="20">
         <v>1</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="21">
         <v>45964</v>
       </c>
-      <c r="J7" s="61" t="b">
+      <c r="J7" s="52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K7" s="60">
+      <c r="K7" s="51">
         <v>45962</v>
       </c>
-      <c r="L7" s="35" t="b">
+      <c r="L7" s="31" t="b">
         <v>1</v>
       </c>
-      <c r="N7" s="37" t="s">
+      <c r="N7" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="38">
+      <c r="O7" s="34">
         <f>AVERAGE(O3:O6)</f>
         <v>89.5</v>
       </c>
-      <c r="P7" s="38">
+      <c r="P7" s="34">
         <f t="shared" ref="P7:Q7" si="5">AVERAGE(P3:P6)</f>
-        <v>13.75</v>
-      </c>
-      <c r="Q7" s="38">
+        <v>15.75</v>
+      </c>
+      <c r="Q7" s="34">
         <f t="shared" si="5"/>
-        <v>75.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>73.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="56"/>
       <c r="B8" s="11">
         <v>3</v>
@@ -3555,56 +3571,56 @@
       <c r="I8" s="13">
         <v>45964</v>
       </c>
-      <c r="J8" s="61" t="b">
+      <c r="J8" s="52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K8" s="59">
+      <c r="K8" s="50">
         <v>45962</v>
       </c>
-      <c r="L8" s="34" t="b">
+      <c r="L8" s="30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="56"/>
-      <c r="B9" s="26">
+      <c r="B9" s="22">
         <v>3</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="22">
         <v>4</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="20">
         <f>IF(F9="","",_xlfn.XLOOKUP(F9,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>8</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="20">
         <v>1</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="21">
         <v>45964</v>
       </c>
-      <c r="J9" s="61" t="b">
+      <c r="J9" s="52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K9" s="60">
+      <c r="K9" s="51">
         <v>45962</v>
       </c>
-      <c r="L9" s="35" t="b">
+      <c r="L9" s="31" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="56"/>
       <c r="B10" s="11">
         <v>3</v>
@@ -3631,58 +3647,58 @@
       <c r="I10" s="13">
         <v>45964</v>
       </c>
-      <c r="J10" s="61" t="b">
+      <c r="J10" s="52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K10" s="59">
+      <c r="K10" s="50">
         <v>45962</v>
       </c>
-      <c r="L10" s="34" t="b">
+      <c r="L10" s="30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
-      <c r="A11" s="27" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="24">
         <v>4</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="24">
         <v>1</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="20">
         <f>IF(F11="","",_xlfn.XLOOKUP(F11,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>8</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="20">
         <v>1</v>
       </c>
-      <c r="I11" s="25">
+      <c r="I11" s="21">
         <v>45964</v>
       </c>
-      <c r="J11" s="61" t="b">
+      <c r="J11" s="52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K11" s="60">
+      <c r="K11" s="51">
         <v>45962</v>
       </c>
-      <c r="L11" s="35" t="b">
+      <c r="L11" s="31" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>35</v>
       </c>
@@ -3711,56 +3727,56 @@
       <c r="I12" s="13">
         <v>45964</v>
       </c>
-      <c r="J12" s="61" t="b">
+      <c r="J12" s="52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K12" s="59">
+      <c r="K12" s="50">
         <v>45962</v>
       </c>
-      <c r="L12" s="34" t="b">
+      <c r="L12" s="30" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="24">
         <v>6</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="24">
         <v>1</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="20">
         <f>IF(F13="","",_xlfn.XLOOKUP(F13,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>8</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="20">
         <v>2</v>
       </c>
-      <c r="I13" s="25">
+      <c r="I13" s="21">
         <v>45978</v>
       </c>
-      <c r="J13" s="61" t="str">
+      <c r="J13" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K13" s="60"/>
-      <c r="L13" s="35" t="b">
+      <c r="K13" s="51"/>
+      <c r="L13" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="54"/>
       <c r="B14" s="11">
         <v>6</v>
@@ -3787,54 +3803,54 @@
       <c r="I14" s="13">
         <v>45978</v>
       </c>
-      <c r="J14" s="61" t="str">
+      <c r="J14" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K14" s="59"/>
-      <c r="L14" s="34" t="b">
+      <c r="K14" s="50"/>
+      <c r="L14" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="24">
         <v>7</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="24">
         <v>1</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="20">
         <f>IF(F15="","",_xlfn.XLOOKUP(F15,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>13</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="20">
         <v>3</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="21">
         <v>45985</v>
       </c>
-      <c r="J15" s="61" t="str">
+      <c r="J15" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K15" s="60"/>
-      <c r="L15" s="35" t="b">
+      <c r="K15" s="51"/>
+      <c r="L15" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="56"/>
       <c r="B16" s="10">
         <v>7</v>
@@ -3861,52 +3877,52 @@
       <c r="I16" s="13">
         <v>45985</v>
       </c>
-      <c r="J16" s="61" t="str">
+      <c r="J16" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K16" s="59"/>
-      <c r="L16" s="34" t="b">
+      <c r="K16" s="50"/>
+      <c r="L16" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="56"/>
-      <c r="B17" s="28">
+      <c r="B17" s="24">
         <v>7</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="22">
         <v>3</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="20">
         <f>IF(F17="","",_xlfn.XLOOKUP(F17,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>13</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="20">
         <v>3</v>
       </c>
-      <c r="I17" s="25">
+      <c r="I17" s="21">
         <v>45985</v>
       </c>
-      <c r="J17" s="61" t="str">
+      <c r="J17" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K17" s="60"/>
-      <c r="L17" s="35" t="b">
+      <c r="K17" s="51"/>
+      <c r="L17" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="56"/>
       <c r="B18" s="10">
         <v>7</v>
@@ -3933,52 +3949,52 @@
       <c r="I18" s="13">
         <v>45985</v>
       </c>
-      <c r="J18" s="61" t="str">
+      <c r="J18" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K18" s="59"/>
-      <c r="L18" s="34" t="b">
+      <c r="K18" s="50"/>
+      <c r="L18" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="56"/>
-      <c r="B19" s="28">
+      <c r="B19" s="24">
         <v>7</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="24">
         <v>5</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="20">
         <f>IF(F19="","",_xlfn.XLOOKUP(F19,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>13</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="20">
         <v>2</v>
       </c>
-      <c r="I19" s="25">
+      <c r="I19" s="21">
         <v>45978</v>
       </c>
-      <c r="J19" s="61" t="str">
+      <c r="J19" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K19" s="60"/>
-      <c r="L19" s="35" t="b">
+      <c r="K19" s="51"/>
+      <c r="L19" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="56"/>
       <c r="B20" s="10">
         <v>7</v>
@@ -4005,52 +4021,52 @@
       <c r="I20" s="13">
         <v>45978</v>
       </c>
-      <c r="J20" s="61" t="str">
+      <c r="J20" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K20" s="59"/>
-      <c r="L20" s="34" t="b">
+      <c r="K20" s="50"/>
+      <c r="L20" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="56"/>
-      <c r="B21" s="28">
+      <c r="B21" s="24">
         <v>7</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="22">
         <v>7</v>
       </c>
-      <c r="D21" s="32" t="s">
+      <c r="D21" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="20">
         <f>IF(F21="","",_xlfn.XLOOKUP(F21,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>8</v>
       </c>
-      <c r="H21" s="24">
+      <c r="H21" s="20">
         <v>3</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="21">
         <v>45985</v>
       </c>
-      <c r="J21" s="61" t="str">
+      <c r="J21" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K21" s="60"/>
-      <c r="L21" s="35" t="b">
+      <c r="K21" s="51"/>
+      <c r="L21" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="56"/>
       <c r="B22" s="10">
         <v>7</v>
@@ -4077,52 +4093,52 @@
       <c r="I22" s="13">
         <v>45985</v>
       </c>
-      <c r="J22" s="61" t="str">
+      <c r="J22" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K22" s="59"/>
-      <c r="L22" s="34" t="b">
+      <c r="K22" s="50"/>
+      <c r="L22" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="56"/>
-      <c r="B23" s="28">
+      <c r="B23" s="24">
         <v>7</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="24">
         <v>9</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="20">
         <f>IF(F23="","",_xlfn.XLOOKUP(F23,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>5</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="20">
         <v>1</v>
       </c>
-      <c r="I23" s="25">
+      <c r="I23" s="21">
         <v>45971</v>
       </c>
-      <c r="J23" s="61" t="str">
+      <c r="J23" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K23" s="60"/>
-      <c r="L23" s="35" t="b">
+      <c r="K23" s="51"/>
+      <c r="L23" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="56"/>
       <c r="B24" s="10">
         <v>7</v>
@@ -4149,52 +4165,52 @@
       <c r="I24" s="13">
         <v>45971</v>
       </c>
-      <c r="J24" s="61" t="str">
+      <c r="J24" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K24" s="59"/>
-      <c r="L24" s="34" t="b">
+      <c r="K24" s="50"/>
+      <c r="L24" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="56"/>
-      <c r="B25" s="28">
+      <c r="B25" s="24">
         <v>7</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="22">
         <v>11</v>
       </c>
-      <c r="D25" s="32" t="s">
+      <c r="D25" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="20">
         <f>IF(F25="","",_xlfn.XLOOKUP(F25,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>13</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="20">
         <v>3</v>
       </c>
-      <c r="I25" s="25">
+      <c r="I25" s="21">
         <v>45978</v>
       </c>
-      <c r="J25" s="61" t="str">
+      <c r="J25" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K25" s="60"/>
-      <c r="L25" s="35" t="b">
+      <c r="K25" s="51"/>
+      <c r="L25" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="56"/>
       <c r="B26" s="10">
         <v>7</v>
@@ -4221,52 +4237,52 @@
       <c r="I26" s="13">
         <v>45971</v>
       </c>
-      <c r="J26" s="61" t="str">
+      <c r="J26" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K26" s="59"/>
-      <c r="L26" s="34" t="b">
+      <c r="K26" s="50"/>
+      <c r="L26" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="56"/>
-      <c r="B27" s="28">
+      <c r="B27" s="24">
         <v>7</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="24">
         <v>13</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="24" t="s">
+      <c r="F27" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="20">
         <f>IF(F27="","",_xlfn.XLOOKUP(F27,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>8</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="20">
         <v>2</v>
       </c>
-      <c r="I27" s="25">
+      <c r="I27" s="21">
         <v>45971</v>
       </c>
-      <c r="J27" s="61" t="str">
+      <c r="J27" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K27" s="60"/>
-      <c r="L27" s="35" t="b">
+      <c r="K27" s="51"/>
+      <c r="L27" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="56"/>
       <c r="B28" s="10">
         <v>7</v>
@@ -4293,52 +4309,52 @@
       <c r="I28" s="13">
         <v>45978</v>
       </c>
-      <c r="J28" s="61" t="str">
+      <c r="J28" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K28" s="59"/>
-      <c r="L28" s="34" t="b">
+      <c r="K28" s="50"/>
+      <c r="L28" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="56"/>
-      <c r="B29" s="28">
+      <c r="B29" s="24">
         <v>7</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="22">
         <v>15</v>
       </c>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="20">
         <f>IF(F29="","",_xlfn.XLOOKUP(F29,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>5</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="20">
         <v>1</v>
       </c>
-      <c r="I29" s="25">
+      <c r="I29" s="21">
         <v>45978</v>
       </c>
-      <c r="J29" s="61" t="str">
+      <c r="J29" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K29" s="60"/>
-      <c r="L29" s="35" t="b">
+      <c r="K29" s="51"/>
+      <c r="L29" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="56"/>
       <c r="B30" s="10">
         <v>7</v>
@@ -4365,52 +4381,52 @@
       <c r="I30" s="13">
         <v>45978</v>
       </c>
-      <c r="J30" s="61" t="str">
+      <c r="J30" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K30" s="59"/>
-      <c r="L30" s="34" t="b">
+      <c r="K30" s="50"/>
+      <c r="L30" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="56"/>
-      <c r="B31" s="28">
+      <c r="B31" s="24">
         <v>7</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="22">
         <v>17</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="20">
         <f>IF(F31="","",_xlfn.XLOOKUP(F31,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>13</v>
       </c>
-      <c r="H31" s="24">
+      <c r="H31" s="20">
         <v>3</v>
       </c>
-      <c r="I31" s="25">
+      <c r="I31" s="21">
         <v>45985</v>
       </c>
-      <c r="J31" s="61" t="str">
+      <c r="J31" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K31" s="60"/>
-      <c r="L31" s="35" t="b">
+      <c r="K31" s="51"/>
+      <c r="L31" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="56"/>
       <c r="B32" s="10">
         <v>7</v>
@@ -4437,52 +4453,52 @@
       <c r="I32" s="13">
         <v>45978</v>
       </c>
-      <c r="J32" s="61" t="str">
+      <c r="J32" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K32" s="59"/>
-      <c r="L32" s="34" t="b">
+      <c r="K32" s="50"/>
+      <c r="L32" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="56"/>
-      <c r="B33" s="28">
+      <c r="B33" s="24">
         <v>7</v>
       </c>
-      <c r="C33" s="28">
+      <c r="C33" s="24">
         <v>19</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="D33" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F33" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="24">
+      <c r="G33" s="20">
         <f>IF(F33="","",_xlfn.XLOOKUP(F33,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>21</v>
       </c>
-      <c r="H33" s="24">
+      <c r="H33" s="20">
         <v>2</v>
       </c>
-      <c r="I33" s="25">
+      <c r="I33" s="21">
         <v>45978</v>
       </c>
-      <c r="J33" s="61" t="str">
+      <c r="J33" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K33" s="60"/>
-      <c r="L33" s="35" t="b">
+      <c r="K33" s="51"/>
+      <c r="L33" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="56"/>
       <c r="B34" s="10">
         <v>7</v>
@@ -4509,56 +4525,56 @@
       <c r="I34" s="13">
         <v>45978</v>
       </c>
-      <c r="J34" s="61" t="str">
+      <c r="J34" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K34" s="59"/>
-      <c r="L34" s="34" t="b">
+      <c r="K34" s="50"/>
+      <c r="L34" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="29.25">
+    <row r="35" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="B35" s="26">
+      <c r="B35" s="22">
         <v>8</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="22">
         <v>1</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="20">
         <f>IF(F35="","",_xlfn.XLOOKUP(F35,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>5</v>
       </c>
-      <c r="H35" s="24">
+      <c r="H35" s="20">
         <v>1</v>
       </c>
-      <c r="I35" s="25">
+      <c r="I35" s="21">
         <v>45971</v>
       </c>
-      <c r="J35" s="61" t="b">
+      <c r="J35" s="52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K35" s="60">
+      <c r="K35" s="51">
         <v>45962</v>
       </c>
-      <c r="L35" s="35" t="b">
+      <c r="L35" s="31" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="54"/>
       <c r="B36" s="11">
         <v>8</v>
@@ -4585,52 +4601,52 @@
       <c r="I36" s="13">
         <v>45971</v>
       </c>
-      <c r="J36" s="61" t="str">
+      <c r="J36" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K36" s="59"/>
-      <c r="L36" s="34" t="b">
+      <c r="K36" s="50"/>
+      <c r="L36" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="54"/>
-      <c r="B37" s="26">
+      <c r="B37" s="22">
         <v>8</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="22">
         <v>3</v>
       </c>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="E37" s="24" t="s">
+      <c r="E37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="24">
+      <c r="G37" s="20">
         <f>IF(F37="","",_xlfn.XLOOKUP(F37,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>8</v>
       </c>
-      <c r="H37" s="24">
+      <c r="H37" s="20">
         <v>1</v>
       </c>
-      <c r="I37" s="25">
+      <c r="I37" s="21">
         <v>45971</v>
       </c>
-      <c r="J37" s="61" t="str">
+      <c r="J37" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K37" s="60"/>
-      <c r="L37" s="35" t="b">
+      <c r="K37" s="51"/>
+      <c r="L37" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="54"/>
       <c r="B38" s="11">
         <v>8</v>
@@ -4657,54 +4673,54 @@
       <c r="I38" s="13">
         <v>45978</v>
       </c>
-      <c r="J38" s="61" t="str">
+      <c r="J38" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K38" s="59"/>
-      <c r="L38" s="34" t="b">
+      <c r="K38" s="50"/>
+      <c r="L38" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="B39" s="26">
+      <c r="B39" s="22">
         <v>9</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="22">
         <v>1</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F39" s="24" t="s">
+      <c r="F39" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="20">
         <f>IF(F39="","",_xlfn.XLOOKUP(F39,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>13</v>
       </c>
-      <c r="H39" s="24">
+      <c r="H39" s="20">
         <v>3</v>
       </c>
-      <c r="I39" s="25">
+      <c r="I39" s="21">
         <v>45985</v>
       </c>
-      <c r="J39" s="61" t="str">
+      <c r="J39" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K39" s="60"/>
-      <c r="L39" s="35" t="b">
+      <c r="K39" s="51"/>
+      <c r="L39" s="31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="55"/>
       <c r="B40" s="11">
         <v>9</v>
@@ -4731,88 +4747,88 @@
       <c r="I40" s="13">
         <v>45985</v>
       </c>
-      <c r="J40" s="61" t="str">
+      <c r="J40" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K40" s="59"/>
-      <c r="L40" s="34" t="b">
+      <c r="K40" s="50"/>
+      <c r="L40" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
-      <c r="D42" s="21"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="D43" s="21"/>
-    </row>
-    <row r="44" spans="1:12">
-      <c r="D44" s="21"/>
-    </row>
-    <row r="45" spans="1:12">
-      <c r="D45" s="21"/>
-    </row>
-    <row r="46" spans="1:12">
-      <c r="D46" s="21"/>
-    </row>
-    <row r="47" spans="1:12">
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="D48" s="21"/>
-    </row>
-    <row r="49" spans="4:4">
-      <c r="D49" s="21"/>
-    </row>
-    <row r="50" spans="4:4">
-      <c r="D50" s="21"/>
-    </row>
-    <row r="51" spans="4:4">
-      <c r="D51" s="21"/>
-    </row>
-    <row r="52" spans="4:4">
-      <c r="D52" s="21"/>
-    </row>
-    <row r="53" spans="4:4">
-      <c r="D53" s="21"/>
-    </row>
-    <row r="54" spans="4:4">
-      <c r="D54" s="21"/>
-    </row>
-    <row r="55" spans="4:4">
-      <c r="D55" s="21"/>
-    </row>
-    <row r="56" spans="4:4">
-      <c r="D56" s="21"/>
-    </row>
-    <row r="57" spans="4:4">
-      <c r="D57" s="21"/>
-    </row>
-    <row r="58" spans="4:4">
-      <c r="D58" s="21"/>
-    </row>
-    <row r="59" spans="4:4">
-      <c r="D59" s="21"/>
-    </row>
-    <row r="60" spans="4:4">
-      <c r="D60" s="21"/>
-    </row>
-    <row r="61" spans="4:4">
-      <c r="D61" s="21"/>
-    </row>
-    <row r="62" spans="4:4">
-      <c r="D62" s="21"/>
-    </row>
-    <row r="63" spans="4:4">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D42" s="17"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D43" s="17"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D44" s="17"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D45" s="17"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D46" s="17"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D47" s="17"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D48" s="17"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="17"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="17"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="17"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="17"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="17"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="17"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="17"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="17"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="17"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="17"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="17"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="17"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="17"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="17"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D63" s="7"/>
     </row>
-    <row r="64" spans="4:4">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D64" s="7"/>
     </row>
-    <row r="65" spans="4:4">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="4:4">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D66" s="7"/>
     </row>
   </sheetData>
@@ -4826,26 +4842,23 @@
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A13:A14"/>
   </mergeCells>
-  <conditionalFormatting sqref="A67:XFD1048576 A43:C66 E43:XFD66 A1:J1 O1:XFD1 L1:M1 A2:XFD42">
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="equal">
-      <formula>"ESSENCIAL"</formula>
+  <conditionalFormatting sqref="A1:J1 L1:M1 O1:XFD1 A2:XFD42 A43:C66 E43:XFD66 A67:XFD1048576">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
+      <formula>"DESEJÁVEL"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:XFD1048576 A43:C66 E43:XFD66 A1:J1 O1:XFD1 L1:M1 A2:XFD42">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"IMPORTANTE"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67:XFD1048576 A43:C66 E43:XFD66 A1:J1 O1:XFD1 L1:M1 A2:XFD42">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
-      <formula>"DESEJÁVEL"</formula>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"ESSENCIAL"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K40" xr:uid="{C0F1E678-E456-4DF2-9AD9-7924FB6139DC}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -4902,7 +4915,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A67:XFD1048576 A43:C66 E43:XFD66 A1:J1 O1:XFD1 L1:M1 A2:XFD42</xm:sqref>
+          <xm:sqref>A1:J1 L1:M1 O1:XFD1 A2:XFD42 A43:C66 E43:XFD66 A67:XFD1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -4952,20 +4965,20 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="17" customFormat="1" ht="18.75">
+    <row r="1" spans="1:6" s="59" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -4978,12 +4991,12 @@
       <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="16"/>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1" s="58"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -5001,7 +5014,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -5019,7 +5032,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -5038,7 +5051,7 @@
       </c>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>20</v>
@@ -5053,7 +5066,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>61</v>
@@ -5066,59 +5079,53 @@
       <c r="E6" s="13"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="13"/>
     </row>
-    <row r="11" spans="1:6" hidden="1">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:6" hidden="1">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="D12" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D11:D12">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="ESSENCIAL">
-      <formula>NOT(ISERROR(SEARCH("ESSENCIAL",D11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A1:E8">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>$E$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>$E$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>$E$4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>$E$5</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E8">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+      <formula>"DESEJÁVEL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"IMPORTANTE"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"ESSENCIAL"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E8">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
-      <formula>"IMPORTANTE"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E8">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
-      <formula>"DESEJÁVEL"</formula>
+  <conditionalFormatting sqref="D11:D12">
+    <cfRule type="containsText" dxfId="0" priority="8" operator="containsText" text="ESSENCIAL">
+      <formula>NOT(ISERROR(SEARCH("ESSENCIAL",D11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
alterei a documentação e o backlog
</commit_message>
<xml_diff>
--- a/BACKLOG - Nippon Insight.xlsx
+++ b/BACKLOG - Nippon Insight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\Projeto Individual\projeto_nippon_insight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC4FA57-C643-4F66-B6AE-B988986134EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6287C0-D89E-407E-9D19-9F3491821491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,9 +17,10 @@
     <sheet name="Listas" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BACKLOG!$A$1:$L$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BACKLOG!$A$1:$L$44</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="75">
   <si>
     <t>REQUISITOS</t>
   </si>
@@ -139,9 +140,6 @@
     <t>G</t>
   </si>
   <si>
-    <t>Objetivo do site</t>
-  </si>
-  <si>
     <t>Como funciona</t>
   </si>
   <si>
@@ -1009,6 +1007,47 @@
         <rFont val="Aptos Narrow"/>
       </rPr>
       <t>roteiro da apresentação:</t>
+    </r>
+  </si>
+  <si>
+    <t>Escopo</t>
+  </si>
+  <si>
+    <t>Determinar a ODS em que o projeto se encaixa</t>
+  </si>
+  <si>
+    <t>Objetivo  e justificativa do site/projeto</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fazer o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>protótipo do dashboard</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fazer o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>protótipo do site</t>
     </r>
   </si>
 </sst>
@@ -1019,7 +1058,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1128,6 +1167,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -1197,7 +1251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1366,6 +1420,16 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1381,10 +1445,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1544,6 +1604,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFCF2F6"/>
       <color rgb="FF0BC1BD"/>
       <color rgb="FF0DDCD7"/>
       <color rgb="FFE46297"/>
@@ -1553,7 +1614,6 @@
       <color rgb="FFFCD62B"/>
       <color rgb="FFD17A0F"/>
       <color rgb="FFFAF1CD"/>
-      <color rgb="FFA3E3E6"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1699,13 +1759,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>358</c:v>
+                  <c:v>403</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>133</c:v>
@@ -1802,10 +1862,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>63</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2569,13 +2629,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1066800</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3151,10 +3211,10 @@
     <tabColor theme="8" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3168,7 +3228,7 @@
     <col min="7" max="7" width="16.5546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="18" style="2" customWidth="1"/>
     <col min="9" max="9" width="17.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" style="2" customWidth="1"/>
     <col min="11" max="11" width="18.44140625" style="2" customWidth="1"/>
     <col min="12" max="12" width="16" style="2" customWidth="1"/>
     <col min="13" max="13" width="9.109375" style="2" customWidth="1"/>
@@ -3207,10 +3267,10 @@
       <c r="I1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="53"/>
+      <c r="K1" s="57"/>
       <c r="L1" s="14" t="s">
         <v>9</v>
       </c>
@@ -3268,19 +3328,19 @@
       </c>
       <c r="O2" s="45">
         <f>SUM(O3:O6)</f>
-        <v>358</v>
+        <v>403</v>
       </c>
       <c r="P2" s="47">
         <f t="shared" ref="P2:Q2" si="0">SUM(P3:P6)</f>
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="Q2" s="49">
         <f t="shared" si="0"/>
-        <v>295</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="18">
@@ -3309,7 +3369,7 @@
         <v>45971</v>
       </c>
       <c r="J3" s="52" t="str">
-        <f t="shared" ref="J3:J40" si="1">IF(K3="","",TRUE)</f>
+        <f t="shared" ref="J3:J44" si="1">IF(K3="","",TRUE)</f>
         <v/>
       </c>
       <c r="K3" s="51"/>
@@ -3320,20 +3380,20 @@
         <v>45964</v>
       </c>
       <c r="O3" s="41">
-        <f>SUMPRODUCT(SUMIF($I$2:$I$40,N3,$G$2:$G$40))</f>
+        <f>SUMPRODUCT(SUMIF($I$2:$I$44,N3,$G$2:$G$44))</f>
         <v>50</v>
       </c>
       <c r="P3" s="41">
-        <f>SUMPRODUCT(SUMIFS($G$2:$G$40,$K$2:$K$40,"&lt;="&amp;N3,$J$2:$J$40,TRUE))</f>
-        <v>63</v>
+        <f>SUMPRODUCT(SUMIFS($G$2:$G$44,$K$2:$K$44,"&lt;="&amp;N3,$J$2:$J$44,TRUE))</f>
+        <v>71</v>
       </c>
       <c r="Q3" s="42">
-        <f>O3-(SUMPRODUCT(SUMIFS($G$2:$G$40,$I$2:$I$40,N3,$J$2:$J$40,TRUE)))</f>
+        <f>O3-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N3,$J$2:$J$44,TRUE)))</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
+      <c r="A4" s="61"/>
       <c r="B4" s="11">
         <v>2</v>
       </c>
@@ -3341,7 +3401,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>15</v>
@@ -3373,20 +3433,20 @@
         <v>45971</v>
       </c>
       <c r="O4" s="43">
-        <f t="shared" ref="O4:O6" si="2">SUMPRODUCT(SUMIF($I$2:$I$40,N4,$G$2:$G$40))</f>
-        <v>68</v>
+        <f>SUMPRODUCT(SUMIF($I$2:$I$44,N4,$G$2:$G$44))</f>
+        <v>113</v>
       </c>
       <c r="P4" s="44">
-        <f>SUMPRODUCT(SUMIFS($G$2:$G$40,$K$2:$K$40,"&gt;"&amp;N3,$K$2:$K$40,"&lt;="&amp;N4,$J$2:$J$40,TRUE))</f>
+        <f>SUMPRODUCT(SUMIFS($G$2:$G$44,$K$2:$K$44,"&gt;"&amp;N3,$K$2:$K$44,"&lt;="&amp;N4,$J$2:$J$44,TRUE))</f>
         <v>0</v>
       </c>
       <c r="Q4" s="44">
-        <f t="shared" ref="Q4:Q6" si="3">O4-(SUMPRODUCT(SUMIFS($G$2:$G$40,$I$2:$I$40,N4,$J$2:$J$40,TRUE)))</f>
-        <v>55</v>
+        <f>O4-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N4,$J$2:$J$44,TRUE)))</f>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
+      <c r="A5" s="61"/>
       <c r="B5" s="22">
         <v>2</v>
       </c>
@@ -3394,176 +3454,174 @@
         <v>3</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G5" s="20">
         <f>IF(F5="","",_xlfn.XLOOKUP(F5,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H5" s="20">
+        <v>1</v>
+      </c>
+      <c r="I5" s="21">
+        <v>45971</v>
+      </c>
+      <c r="J5" s="52" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K5" s="51">
+        <v>45964</v>
+      </c>
+      <c r="L5" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="13">
+        <v>45978</v>
+      </c>
+      <c r="O5" s="38">
+        <f>SUMPRODUCT(SUMIF($I$2:$I$44,N5,$G$2:$G$44))</f>
+        <v>133</v>
+      </c>
+      <c r="P5" s="39">
+        <f>SUMPRODUCT(SUMIFS($G$2:$G$44,$K$2:$K$44,"&gt;"&amp;N4,$K$2:$K$44,"&lt;="&amp;N5,$J$2:$J$44,TRUE))</f>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="39">
+        <f>O5-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N5,$J$2:$J$44,TRUE)))</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="61"/>
+      <c r="B6" s="11">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="2">
+        <f>IF(F6="","",_xlfn.XLOOKUP(F6,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>3</v>
       </c>
-      <c r="I5" s="21">
-        <v>45978</v>
-      </c>
-      <c r="J5" s="52" t="str">
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" s="13">
+        <v>45971</v>
+      </c>
+      <c r="J6" s="52" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K5" s="51"/>
-      <c r="L5" s="31" t="b">
+      <c r="K6" s="50"/>
+      <c r="L6" s="30" t="b">
         <v>0</v>
-      </c>
-      <c r="N5" s="13">
-        <v>45978</v>
-      </c>
-      <c r="O5" s="38">
-        <f>SUMPRODUCT(SUMIF($I$2:$I$40,N5,$G$2:$G$40))</f>
-        <v>133</v>
-      </c>
-      <c r="P5" s="39">
-        <f t="shared" ref="P5:P6" si="4">SUMPRODUCT(SUMIFS($G$2:$G$40,$K$2:$K$40,"&gt;"&amp;N4,$K$2:$K$40,"&lt;="&amp;N5,$J$2:$J$40,TRUE))</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="39">
-        <f t="shared" si="3"/>
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="11">
-        <v>3</v>
-      </c>
-      <c r="C6" s="11">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="2">
-        <f>IF(F6="","",_xlfn.XLOOKUP(F6,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="13">
-        <v>45964</v>
-      </c>
-      <c r="J6" s="52" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K6" s="50">
-        <v>45962</v>
-      </c>
-      <c r="L6" s="30" t="b">
-        <v>1</v>
       </c>
       <c r="N6" s="13">
         <v>45985</v>
       </c>
       <c r="O6" s="36">
-        <f t="shared" si="2"/>
+        <f>SUMPRODUCT(SUMIF($I$2:$I$44,N6,$G$2:$G$44))</f>
         <v>107</v>
       </c>
       <c r="P6" s="37">
-        <f t="shared" si="4"/>
+        <f>SUMPRODUCT(SUMIFS($G$2:$G$44,$K$2:$K$44,"&gt;"&amp;N5,$K$2:$K$44,"&lt;="&amp;N6,$J$2:$J$44,TRUE))</f>
         <v>0</v>
       </c>
       <c r="Q6" s="37">
-        <f t="shared" si="3"/>
+        <f>O6-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N6,$J$2:$J$44,TRUE)))</f>
         <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="56"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="22">
-        <v>2</v>
-      </c>
-      <c r="D7" s="25" t="s">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G7" s="20">
         <f>IF(F7="","",_xlfn.XLOOKUP(F7,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
         <v>5</v>
       </c>
       <c r="H7" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I7" s="21">
-        <v>45964</v>
-      </c>
-      <c r="J7" s="52" t="b">
+        <v>45978</v>
+      </c>
+      <c r="J7" s="52" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K7" s="51">
-        <v>45962</v>
-      </c>
+        <v/>
+      </c>
+      <c r="K7" s="51"/>
       <c r="L7" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O7" s="34">
         <f>AVERAGE(O3:O6)</f>
-        <v>89.5</v>
+        <v>100.75</v>
       </c>
       <c r="P7" s="34">
-        <f t="shared" ref="P7:Q7" si="5">AVERAGE(P3:P6)</f>
-        <v>15.75</v>
+        <f t="shared" ref="P7:Q7" si="2">AVERAGE(P3:P6)</f>
+        <v>17.75</v>
       </c>
       <c r="Q7" s="34">
-        <f t="shared" si="5"/>
-        <v>73.75</v>
+        <f t="shared" si="2"/>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8" s="56"/>
+      <c r="A8" s="60" t="s">
+        <v>24</v>
+      </c>
       <c r="B8" s="11">
         <v>3</v>
       </c>
       <c r="C8" s="11">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G8" s="2">
         <f>IF(F8="","",_xlfn.XLOOKUP(F8,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -3583,25 +3641,25 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="56"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="22">
         <v>3</v>
       </c>
       <c r="C9" s="22">
-        <v>4</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>31</v>
+        <v>2</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G9" s="20">
         <f>IF(F9="","",_xlfn.XLOOKUP(F9,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H9" s="20">
         <v>1</v>
@@ -3621,25 +3679,25 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="56"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="11">
         <v>3</v>
       </c>
       <c r="C10" s="11">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G10" s="2">
         <f>IF(F10="","",_xlfn.XLOOKUP(F10,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H10" s="2">
         <v>1</v>
@@ -3659,20 +3717,18 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="24">
+      <c r="A11" s="60"/>
+      <c r="B11" s="22">
+        <v>3</v>
+      </c>
+      <c r="C11" s="22">
         <v>4</v>
       </c>
-      <c r="C11" s="24">
-        <v>1</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>34</v>
+      <c r="D11" s="27" t="s">
+        <v>30</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>16</v>
@@ -3699,27 +3755,25 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="10">
+      <c r="A12" s="60"/>
+      <c r="B12" s="11">
+        <v>3</v>
+      </c>
+      <c r="C12" s="11">
         <v>5</v>
       </c>
-      <c r="C12" s="10">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>36</v>
+      <c r="D12" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="G12" s="2">
         <f>IF(F12="","",_xlfn.XLOOKUP(F12,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H12" s="2">
         <v>1</v>
@@ -3739,20 +3793,20 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="54" t="s">
-        <v>38</v>
+      <c r="A13" s="23" t="s">
+        <v>32</v>
       </c>
       <c r="B13" s="24">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C13" s="24">
         <v>1</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>39</v>
+      <c r="D13" s="19" t="s">
+        <v>33</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="20" t="s">
         <v>16</v>
@@ -3762,87 +3816,93 @@
         <v>8</v>
       </c>
       <c r="H13" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="21">
-        <v>45978</v>
-      </c>
-      <c r="J13" s="52" t="str">
+        <v>45964</v>
+      </c>
+      <c r="J13" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K13" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K13" s="51">
+        <v>45962</v>
+      </c>
       <c r="L13" s="31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="11">
-        <v>6</v>
-      </c>
-      <c r="C14" s="11">
-        <v>2</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>40</v>
+      <c r="A14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="10">
+        <v>5</v>
+      </c>
+      <c r="C14" s="10">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="G14" s="2">
         <f>IF(F14="","",_xlfn.XLOOKUP(F14,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="13">
-        <v>45978</v>
-      </c>
-      <c r="J14" s="52" t="str">
+        <v>45964</v>
+      </c>
+      <c r="J14" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K14" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K14" s="50">
+        <v>45962</v>
+      </c>
       <c r="L14" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
-        <v>41</v>
+      <c r="A15" s="58" t="s">
+        <v>37</v>
       </c>
       <c r="B15" s="24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="24">
         <v>1</v>
       </c>
       <c r="D15" s="25" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G15" s="20">
         <f>IF(F15="","",_xlfn.XLOOKUP(F15,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H15" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15" s="21">
-        <v>45985</v>
+        <v>45978</v>
       </c>
       <c r="J15" s="52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J15:J16" si="3">IF(K15="","",TRUE)</f>
         <v/>
       </c>
       <c r="K15" s="51"/>
@@ -3851,34 +3911,34 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="56"/>
-      <c r="B16" s="10">
-        <v>7</v>
+      <c r="A16" s="58"/>
+      <c r="B16" s="11">
+        <v>6</v>
       </c>
       <c r="C16" s="11">
         <v>2</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>43</v>
+      <c r="D16" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G16" s="2">
         <f>IF(F16="","",_xlfn.XLOOKUP(F16,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I16" s="13">
-        <v>45985</v>
+        <v>45978</v>
       </c>
       <c r="J16" s="52" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K16" s="50"/>
@@ -3887,18 +3947,18 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="56"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="24">
-        <v>7</v>
-      </c>
-      <c r="C17" s="22">
+        <v>6</v>
+      </c>
+      <c r="C17" s="24">
         <v>3</v>
       </c>
-      <c r="D17" s="28" t="s">
-        <v>44</v>
+      <c r="D17" s="55" t="s">
+        <v>73</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>20</v>
@@ -3908,10 +3968,10 @@
         <v>13</v>
       </c>
       <c r="H17" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I17" s="21">
-        <v>45985</v>
+        <v>45971</v>
       </c>
       <c r="J17" s="52" t="str">
         <f t="shared" si="1"/>
@@ -3923,31 +3983,33 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="56"/>
-      <c r="B18" s="10">
+      <c r="A18" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="11">
         <v>7</v>
       </c>
       <c r="C18" s="11">
-        <v>4</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>45</v>
+        <v>1</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G18" s="2">
         <f>IF(F18="","",_xlfn.XLOOKUP(F18,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I18" s="13">
-        <v>45985</v>
+        <v>45971</v>
       </c>
       <c r="J18" s="52" t="str">
         <f t="shared" si="1"/>
@@ -3959,18 +4021,18 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="56"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="24">
         <v>7</v>
       </c>
       <c r="C19" s="24">
-        <v>5</v>
-      </c>
-      <c r="D19" s="29" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>41</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>20</v>
@@ -3980,10 +4042,10 @@
         <v>13</v>
       </c>
       <c r="H19" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19" s="21">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="J19" s="52" t="str">
         <f t="shared" si="1"/>
@@ -3995,18 +4057,18 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="56"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="10">
         <v>7</v>
       </c>
       <c r="C20" s="11">
-        <v>6</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>47</v>
+        <v>3</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>20</v>
@@ -4016,10 +4078,10 @@
         <v>13</v>
       </c>
       <c r="H20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I20" s="13">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="J20" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4031,25 +4093,25 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="56"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="24">
         <v>7</v>
       </c>
       <c r="C21" s="22">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G21" s="20">
         <f>IF(F21="","",_xlfn.XLOOKUP(F21,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H21" s="20">
         <v>3</v>
@@ -4067,18 +4129,18 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="56"/>
+      <c r="A22" s="60"/>
       <c r="B22" s="10">
         <v>7</v>
       </c>
       <c r="C22" s="11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>20</v>
@@ -4103,31 +4165,31 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="56"/>
+      <c r="A23" s="60"/>
       <c r="B23" s="24">
         <v>7</v>
       </c>
       <c r="C23" s="24">
-        <v>9</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>50</v>
+        <v>6</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>45</v>
       </c>
       <c r="E23" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G23" s="20">
         <f>IF(F23="","",_xlfn.XLOOKUP(F23,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H23" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="21">
-        <v>45971</v>
+        <v>45978</v>
       </c>
       <c r="J23" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4139,31 +4201,31 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="56"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="10">
         <v>7</v>
       </c>
       <c r="C24" s="11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G24" s="2">
         <f>IF(F24="","",_xlfn.XLOOKUP(F24,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H24" s="2">
         <v>2</v>
       </c>
       <c r="I24" s="13">
-        <v>45971</v>
+        <v>45978</v>
       </c>
       <c r="J24" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4175,31 +4237,31 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="56"/>
+      <c r="A25" s="60"/>
       <c r="B25" s="24">
         <v>7</v>
       </c>
       <c r="C25" s="22">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F25" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G25" s="20">
         <f>IF(F25="","",_xlfn.XLOOKUP(F25,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H25" s="20">
         <v>3</v>
       </c>
       <c r="I25" s="21">
-        <v>45978</v>
+        <v>45985</v>
       </c>
       <c r="J25" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4211,31 +4273,31 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="56"/>
+      <c r="A26" s="60"/>
       <c r="B26" s="10">
         <v>7</v>
       </c>
       <c r="C26" s="11">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G26" s="2">
         <f>IF(F26="","",_xlfn.XLOOKUP(F26,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H26" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26" s="13">
-        <v>45971</v>
+        <v>45985</v>
       </c>
       <c r="J26" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4247,28 +4309,28 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="56"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="24">
         <v>7</v>
       </c>
       <c r="C27" s="24">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G27" s="20">
         <f>IF(F27="","",_xlfn.XLOOKUP(F27,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H27" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="21">
         <v>45971</v>
@@ -4283,31 +4345,31 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="56"/>
+      <c r="A28" s="60"/>
       <c r="B28" s="10">
         <v>7</v>
       </c>
       <c r="C28" s="11">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G28" s="2">
         <f>IF(F28="","",_xlfn.XLOOKUP(F28,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H28" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I28" s="13">
-        <v>45978</v>
+        <v>45971</v>
       </c>
       <c r="J28" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4319,28 +4381,28 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="56"/>
+      <c r="A29" s="60"/>
       <c r="B29" s="24">
         <v>7</v>
       </c>
       <c r="C29" s="22">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G29" s="20">
         <f>IF(F29="","",_xlfn.XLOOKUP(F29,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H29" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I29" s="21">
         <v>45978</v>
@@ -4355,31 +4417,31 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="56"/>
+      <c r="A30" s="60"/>
       <c r="B30" s="10">
         <v>7</v>
       </c>
-      <c r="C30" s="10">
-        <v>16</v>
+      <c r="C30" s="11">
+        <v>13</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G30" s="2">
         <f>IF(F30="","",_xlfn.XLOOKUP(F30,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H30" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30" s="13">
-        <v>45978</v>
+        <v>45971</v>
       </c>
       <c r="J30" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4391,31 +4453,31 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="56"/>
+      <c r="A31" s="60"/>
       <c r="B31" s="24">
         <v>7</v>
       </c>
-      <c r="C31" s="22">
-        <v>17</v>
+      <c r="C31" s="24">
+        <v>14</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G31" s="20">
         <f>IF(F31="","",_xlfn.XLOOKUP(F31,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H31" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I31" s="21">
-        <v>45985</v>
+        <v>45971</v>
       </c>
       <c r="J31" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4427,28 +4489,28 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="56"/>
+      <c r="A32" s="60"/>
       <c r="B32" s="10">
         <v>7</v>
       </c>
       <c r="C32" s="11">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G32" s="2">
         <f>IF(F32="","",_xlfn.XLOOKUP(F32,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H32" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I32" s="13">
         <v>45978</v>
@@ -4463,28 +4525,28 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="56"/>
+      <c r="A33" s="60"/>
       <c r="B33" s="24">
         <v>7</v>
       </c>
-      <c r="C33" s="24">
-        <v>19</v>
+      <c r="C33" s="22">
+        <v>16</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F33" s="20" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="G33" s="20">
         <f>IF(F33="","",_xlfn.XLOOKUP(F33,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H33" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I33" s="21">
         <v>45978</v>
@@ -4499,28 +4561,28 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="56"/>
+      <c r="A34" s="60"/>
       <c r="B34" s="10">
         <v>7</v>
       </c>
-      <c r="C34" s="11">
-        <v>20</v>
+      <c r="C34" s="10">
+        <v>17</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="G34" s="2">
         <f>IF(F34="","",_xlfn.XLOOKUP(F34,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H34" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I34" s="13">
         <v>45978</v>
@@ -4534,72 +4596,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="B35" s="22">
-        <v>8</v>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="60"/>
+      <c r="B35" s="24">
+        <v>7</v>
       </c>
       <c r="C35" s="22">
-        <v>1</v>
-      </c>
-      <c r="D35" s="26" t="s">
-        <v>64</v>
+        <v>18</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>57</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G35" s="20">
         <f>IF(F35="","",_xlfn.XLOOKUP(F35,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H35" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I35" s="21">
-        <v>45971</v>
-      </c>
-      <c r="J35" s="52" t="b">
+        <v>45985</v>
+      </c>
+      <c r="J35" s="52" t="str">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K35" s="51">
-        <v>45962</v>
-      </c>
+        <v/>
+      </c>
+      <c r="K35" s="51"/>
       <c r="L35" s="31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="54"/>
-      <c r="B36" s="11">
-        <v>8</v>
+      <c r="A36" s="60"/>
+      <c r="B36" s="10">
+        <v>7</v>
       </c>
       <c r="C36" s="11">
-        <v>2</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>65</v>
+        <v>19</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G36" s="2">
         <f>IF(F36="","",_xlfn.XLOOKUP(F36,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H36" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="13">
-        <v>45971</v>
+        <v>45978</v>
       </c>
       <c r="J36" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4611,31 +4669,31 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="54"/>
-      <c r="B37" s="22">
-        <v>8</v>
-      </c>
-      <c r="C37" s="22">
-        <v>3</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>66</v>
+      <c r="A37" s="60"/>
+      <c r="B37" s="24">
+        <v>7</v>
+      </c>
+      <c r="C37" s="24">
+        <v>20</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>59</v>
       </c>
       <c r="E37" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F37" s="20" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G37" s="20">
         <f>IF(F37="","",_xlfn.XLOOKUP(F37,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="H37" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I37" s="21">
-        <v>45971</v>
+        <v>45978</v>
       </c>
       <c r="J37" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4647,25 +4705,25 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="54"/>
-      <c r="B38" s="11">
-        <v>8</v>
+      <c r="A38" s="60"/>
+      <c r="B38" s="10">
+        <v>7</v>
       </c>
       <c r="C38" s="11">
-        <v>4</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>67</v>
+        <v>21</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G38" s="2">
         <f>IF(F38="","",_xlfn.XLOOKUP(F38,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H38" s="2">
         <v>3</v>
@@ -4682,54 +4740,56 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="55" t="s">
-        <v>68</v>
+    <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="58" t="s">
+        <v>62</v>
       </c>
       <c r="B39" s="22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C39" s="22">
         <v>1</v>
       </c>
-      <c r="D39" s="25" t="s">
-        <v>69</v>
+      <c r="D39" s="26" t="s">
+        <v>63</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G39" s="20">
         <f>IF(F39="","",_xlfn.XLOOKUP(F39,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H39" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I39" s="21">
-        <v>45985</v>
-      </c>
-      <c r="J39" s="52" t="str">
+        <v>45971</v>
+      </c>
+      <c r="J39" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K39" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K39" s="51">
+        <v>45962</v>
+      </c>
       <c r="L39" s="31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="55"/>
+      <c r="A40" s="58"/>
       <c r="B40" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" s="11">
         <v>2</v>
       </c>
-      <c r="D40" s="7" t="s">
-        <v>70</v>
+      <c r="D40" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>15</v>
@@ -4742,10 +4802,10 @@
         <v>8</v>
       </c>
       <c r="H40" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I40" s="13">
-        <v>45985</v>
+        <v>45971</v>
       </c>
       <c r="J40" s="52" t="str">
         <f t="shared" si="1"/>
@@ -4756,17 +4816,151 @@
         <v>0</v>
       </c>
     </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="58"/>
+      <c r="B41" s="22">
+        <v>8</v>
+      </c>
+      <c r="C41" s="22">
+        <v>3</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" s="20">
+        <f>IF(F41="","",_xlfn.XLOOKUP(F41,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
+        <v>8</v>
+      </c>
+      <c r="H41" s="20">
+        <v>1</v>
+      </c>
+      <c r="I41" s="21">
+        <v>45971</v>
+      </c>
+      <c r="J41" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K41" s="51"/>
+      <c r="L41" s="31" t="b">
+        <v>0</v>
+      </c>
+    </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D42" s="17"/>
+      <c r="A42" s="58"/>
+      <c r="B42" s="11">
+        <v>8</v>
+      </c>
+      <c r="C42" s="11">
+        <v>4</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" s="2">
+        <f>IF(F42="","",_xlfn.XLOOKUP(F42,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
+        <v>8</v>
+      </c>
+      <c r="H42" s="2">
+        <v>3</v>
+      </c>
+      <c r="I42" s="13">
+        <v>45978</v>
+      </c>
+      <c r="J42" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K42" s="50"/>
+      <c r="L42" s="30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D43" s="17"/>
+      <c r="A43" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="22">
+        <v>9</v>
+      </c>
+      <c r="C43" s="22">
+        <v>1</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="20">
+        <f>IF(F43="","",_xlfn.XLOOKUP(F43,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
+        <v>13</v>
+      </c>
+      <c r="H43" s="20">
+        <v>3</v>
+      </c>
+      <c r="I43" s="21">
+        <v>45985</v>
+      </c>
+      <c r="J43" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K43" s="51"/>
+      <c r="L43" s="31" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D44" s="17"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="D45" s="17"/>
+      <c r="A44" s="59"/>
+      <c r="B44" s="11">
+        <v>9</v>
+      </c>
+      <c r="C44" s="11">
+        <v>2</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" s="2">
+        <f>IF(F44="","",_xlfn.XLOOKUP(F44,Listas!$B$2:$B$7,Listas!$C$2:$C$7))</f>
+        <v>8</v>
+      </c>
+      <c r="H44" s="2">
+        <v>3</v>
+      </c>
+      <c r="I44" s="13">
+        <v>45985</v>
+      </c>
+      <c r="J44" s="52" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K44" s="50"/>
+      <c r="L44" s="30" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D46" s="17"/>
@@ -4820,29 +5014,41 @@
       <c r="D62" s="17"/>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D63" s="7"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D64" s="7"/>
+      <c r="D64" s="17"/>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D65" s="7"/>
+      <c r="D65" s="17"/>
     </row>
     <row r="66" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D66" s="7"/>
+      <c r="D66" s="17"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="7"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L40" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L44" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="7">
     <mergeCell ref="J1:K1"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A15:A34"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A38"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:J1 L1:M1 O1:XFD1 A2:XFD42 A43:C66 E43:XFD66 A67:XFD1048576">
+  <conditionalFormatting sqref="A1:J1 L1:M1 O1:XFD1 A2:XFD3 B4:XFD4 B5:I7 J5:L8 M5:XFD1048576 A8:I8 A9:L15 B16:L17 A18:L18 B19:L38 A39:L46 A47:C70 E47:L70 A71:L1048576">
     <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
       <formula>"DESEJÁVEL"</formula>
     </cfRule>
@@ -4854,7 +5060,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K40" xr:uid="{C0F1E678-E456-4DF2-9AD9-7924FB6139DC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K44" xr:uid="{C0F1E678-E456-4DF2-9AD9-7924FB6139DC}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" orientation="landscape" r:id="rId1"/>
@@ -4915,41 +5121,41 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A1:J1 L1:M1 O1:XFD1 A2:XFD42 A43:C66 E43:XFD66 A67:XFD1048576</xm:sqref>
+          <xm:sqref>A1:J1 L1:M1 O1:XFD1 A2:XFD3 B4:XFD4 B5:I7 J5:L8 M5:XFD1048576 A8:I8 A9:L15 B16:L17 A18:L18 B19:L38 A39:L46 A47:C70 E47:L70 A71:L1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3BCB1527-7317-4D7E-A692-125B8FD6118D}">
+          <x14:formula1>
+            <xm:f>Listas!$E$2:$E$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>N3:N6</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{503E7DAE-EDB6-474F-864E-716F9D882DAF}">
           <x14:formula1>
             <xm:f>Listas!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E40</xm:sqref>
+          <xm:sqref>E2:E44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{904B9BC7-BA26-49A5-8221-8302483833B8}">
           <x14:formula1>
             <xm:f>Listas!$B$2:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F40</xm:sqref>
+          <xm:sqref>F2:F44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{846C7866-2918-42E4-B1C8-871ACF497667}">
           <x14:formula1>
             <xm:f>Listas!$D$2:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H40</xm:sqref>
+          <xm:sqref>H2:H44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{281048C2-2B84-4EDD-A65D-F93F61361462}">
           <x14:formula1>
             <xm:f>Listas!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I40</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3BCB1527-7317-4D7E-A692-125B8FD6118D}">
-          <x14:formula1>
-            <xm:f>Listas!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>N3:N6</xm:sqref>
+          <xm:sqref>I2:I44</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4978,7 +5184,7 @@
     <col min="6" max="6" width="10.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="59" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="54" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
@@ -4994,14 +5200,14 @@
       <c r="E1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="58"/>
+      <c r="F1" s="53"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
@@ -5016,10 +5222,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -5034,7 +5240,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>16</v>
@@ -5069,7 +5275,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
backlog atualizado e upload do web-data-viz
</commit_message>
<xml_diff>
--- a/BACKLOG - Nippon Insight.xlsx
+++ b/BACKLOG - Nippon Insight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\Projeto Individual\projeto_nippon_insight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6287C0-D89E-407E-9D19-9F3491821491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E710222-786B-4AAC-99BC-DFC2E8194242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BACKLOG!$A$1:$L$44</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1862,13 +1861,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>71</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3214,7 +3213,7 @@
   <dimension ref="A1:Q70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3332,11 +3331,11 @@
       </c>
       <c r="P2" s="47">
         <f t="shared" ref="P2:Q2" si="0">SUM(P3:P6)</f>
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="Q2" s="49">
         <f t="shared" si="0"/>
-        <v>332</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -3438,11 +3437,11 @@
       </c>
       <c r="P4" s="44">
         <f>SUMPRODUCT(SUMIFS($G$2:$G$44,$K$2:$K$44,"&gt;"&amp;N3,$K$2:$K$44,"&lt;="&amp;N4,$J$2:$J$44,TRUE))</f>
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="Q4" s="44">
         <f>O4-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N4,$J$2:$J$44,TRUE)))</f>
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3525,11 +3524,13 @@
       <c r="I6" s="13">
         <v>45971</v>
       </c>
-      <c r="J6" s="52" t="str">
+      <c r="J6" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K6" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K6" s="50">
+        <v>45968</v>
+      </c>
       <c r="L6" s="30" t="b">
         <v>0</v>
       </c>
@@ -3593,11 +3594,11 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" ref="P7:Q7" si="2">AVERAGE(P3:P6)</f>
-        <v>17.75</v>
+        <v>22.5</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="2"/>
-        <v>83</v>
+        <v>78.25</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -4807,11 +4808,13 @@
       <c r="I40" s="13">
         <v>45971</v>
       </c>
-      <c r="J40" s="52" t="str">
+      <c r="J40" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K40" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K40" s="50">
+        <v>45970</v>
+      </c>
       <c r="L40" s="30" t="b">
         <v>0</v>
       </c>
@@ -4843,11 +4846,13 @@
       <c r="I41" s="21">
         <v>45971</v>
       </c>
-      <c r="J41" s="52" t="str">
+      <c r="J41" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K41" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K41" s="51">
+        <v>45970</v>
+      </c>
       <c r="L41" s="31" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Update Doc, Backlog, site
</commit_message>
<xml_diff>
--- a/BACKLOG - Nippon Insight.xlsx
+++ b/BACKLOG - Nippon Insight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\Projeto Individual\projeto_nippon_insight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC8ABE7-E63C-4715-86A7-9FDF0779C658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BCD396-E95A-46A9-B3F3-2853707C4119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>179</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>71</c:v>
@@ -1870,7 +1870,7 @@
                   <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3212,8 +3212,8 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3331,11 +3331,11 @@
       </c>
       <c r="P2" s="47">
         <f t="shared" ref="P2:Q2" si="0">SUM(P3:P6)</f>
-        <v>179</v>
+        <v>218</v>
       </c>
       <c r="Q2" s="49">
         <f t="shared" si="0"/>
-        <v>224</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -3492,11 +3492,11 @@
       </c>
       <c r="P5" s="39">
         <f>SUMPRODUCT(SUMIFS($G$2:$G$44,$K$2:$K$44,"&gt;"&amp;N4,$K$2:$K$44,"&lt;="&amp;N5,$J$2:$J$44,TRUE))</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="39">
         <f>O5-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N5,$J$2:$J$44,TRUE)))</f>
-        <v>117</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3549,7 +3549,7 @@
       </c>
       <c r="Q6" s="37">
         <f>O6-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N6,$J$2:$J$44,TRUE)))</f>
-        <v>81</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
@@ -3596,11 +3596,11 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" ref="P7:Q7" si="2">AVERAGE(P3:P6)</f>
-        <v>44.75</v>
+        <v>54.5</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v>46.25</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -4094,11 +4094,13 @@
       <c r="I20" s="13">
         <v>45985</v>
       </c>
-      <c r="J20" s="52" t="str">
+      <c r="J20" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K20" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="50">
+        <v>45974</v>
+      </c>
       <c r="L20" s="30" t="b">
         <v>0</v>
       </c>
@@ -4422,11 +4424,13 @@
       <c r="I29" s="21">
         <v>45978</v>
       </c>
-      <c r="J29" s="52" t="str">
+      <c r="J29" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K29" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K29" s="51">
+        <v>45974</v>
+      </c>
       <c r="L29" s="31" t="b">
         <v>0</v>
       </c>
@@ -4534,11 +4538,13 @@
       <c r="I32" s="13">
         <v>45978</v>
       </c>
-      <c r="J32" s="52" t="str">
+      <c r="J32" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K32" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K32" s="50">
+        <v>45974</v>
+      </c>
       <c r="L32" s="30" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
site com login e senha funcionando
</commit_message>
<xml_diff>
--- a/BACKLOG - Nippon Insight.xlsx
+++ b/BACKLOG - Nippon Insight.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\Projeto Individual\projeto_nippon_insight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BCD396-E95A-46A9-B3F3-2853707C4119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7E6C9FF-C113-402E-AD66-06EB9156420F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1861,7 +1861,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>218</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>71</c:v>
@@ -1870,7 +1870,7 @@
                   <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -3212,8 +3212,8 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3331,11 +3331,11 @@
       </c>
       <c r="P2" s="47">
         <f t="shared" ref="P2:Q2" si="0">SUM(P3:P6)</f>
-        <v>218</v>
+        <v>249</v>
       </c>
       <c r="Q2" s="49">
         <f t="shared" si="0"/>
-        <v>185</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="Q4" s="44">
         <f>O4-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N4,$J$2:$J$44,TRUE)))</f>
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3492,11 +3492,11 @@
       </c>
       <c r="P5" s="39">
         <f>SUMPRODUCT(SUMIFS($G$2:$G$44,$K$2:$K$44,"&gt;"&amp;N4,$K$2:$K$44,"&lt;="&amp;N5,$J$2:$J$44,TRUE))</f>
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="Q5" s="39">
         <f>O5-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N5,$J$2:$J$44,TRUE)))</f>
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3596,11 +3596,11 @@
       </c>
       <c r="P7" s="34">
         <f t="shared" ref="P7:Q7" si="2">AVERAGE(P3:P6)</f>
-        <v>54.5</v>
+        <v>62.25</v>
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="2"/>
-        <v>46.25</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -4350,11 +4350,13 @@
       <c r="I27" s="21">
         <v>45971</v>
       </c>
-      <c r="J27" s="52" t="str">
+      <c r="J27" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K27" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K27" s="51">
+        <v>45977</v>
+      </c>
       <c r="L27" s="31" t="b">
         <v>0</v>
       </c>
@@ -4684,11 +4686,13 @@
       <c r="I36" s="13">
         <v>45978</v>
       </c>
-      <c r="J36" s="52" t="str">
+      <c r="J36" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K36" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K36" s="50">
+        <v>45977</v>
+      </c>
       <c r="L36" s="30" t="b">
         <v>0</v>
       </c>
@@ -4756,11 +4760,13 @@
       <c r="I38" s="13">
         <v>45978</v>
       </c>
-      <c r="J38" s="52" t="str">
+      <c r="J38" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K38" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K38" s="50">
+        <v>45977</v>
+      </c>
       <c r="L38" s="30" t="b">
         <v>0</v>
       </c>
@@ -4908,11 +4914,13 @@
       <c r="I42" s="13">
         <v>45978</v>
       </c>
-      <c r="J42" s="52" t="str">
+      <c r="J42" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K42" s="50"/>
+        <v>1</v>
+      </c>
+      <c r="K42" s="50">
+        <v>45977</v>
+      </c>
       <c r="L42" s="30" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
atualização do backlog e da documentação
</commit_message>
<xml_diff>
--- a/BACKLOG - Nippon Insight.xlsx
+++ b/BACKLOG - Nippon Insight.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\Projeto Individual\projeto_nippon_insight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amiyu\Documents\GitHub - Repositórios\projeto_nippon_insight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A81D5-63C6-47C9-A1E0-E183A85C51A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D3F9BC-A625-42AC-A72C-D7551C59331C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3212,8 +3212,8 @@
   </sheetPr>
   <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3335,7 +3335,7 @@
       </c>
       <c r="Q2" s="49">
         <f t="shared" si="0"/>
-        <v>154</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -3496,7 +3496,7 @@
       </c>
       <c r="Q5" s="39">
         <f>O5-(SUMPRODUCT(SUMIFS($G$2:$G$44,$I$2:$I$44,N5,$J$2:$J$44,TRUE)))</f>
-        <v>65</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3600,7 +3600,7 @@
       </c>
       <c r="Q7" s="34">
         <f t="shared" si="2"/>
-        <v>38.5</v>
+        <v>33.25</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -4005,7 +4005,7 @@
         <v>74</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>60</v>
@@ -4155,7 +4155,7 @@
         <v>44</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>20</v>
@@ -4191,7 +4191,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F23" s="20" t="s">
         <v>20</v>
@@ -4724,11 +4724,13 @@
       <c r="I37" s="21">
         <v>45978</v>
       </c>
-      <c r="J37" s="52" t="str">
+      <c r="J37" s="52" t="b">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K37" s="51"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="51">
+        <v>45986</v>
+      </c>
       <c r="L37" s="31" t="b">
         <v>0</v>
       </c>

</xml_diff>